<commit_message>
updated outputs with single child
</commit_message>
<xml_diff>
--- a/outputs-HGR-r202/c__Clostridia_A.xlsx
+++ b/outputs-HGR-r202/c__Clostridia_A.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,15 +447,10 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>max</t>
+          <t>prediction</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>prediction</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>rejection-f</t>
         </is>
@@ -468,17 +463,14 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
+        <v>95809.76437652647</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -487,21 +479,18 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT10635.fa</t>
+          <t>even_MAG-GUT22878.fa</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
+        <v>84300.51216472185</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -510,21 +499,18 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT1707.fa</t>
+          <t>even_MAG-GUT28136.fa</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
+        <v>81207.03595207828</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -533,21 +519,18 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT22878.fa</t>
+          <t>even_MAG-GUT29051.fa</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
+        <v>73972.36771533091</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -556,21 +539,18 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT28136.fa</t>
+          <t>even_MAG-GUT29076.fa</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
+        <v>83485.85692499307</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -579,21 +559,18 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT29051.fa</t>
+          <t>even_MAG-GUT40857.fa</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
+        <v>66602.25207459994</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D7" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -602,21 +579,18 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT29076.fa</t>
+          <t>even_MAG-GUT42485.fa</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
+        <v>77062.31740954959</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D8" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -625,21 +599,18 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT40857.fa</t>
+          <t>even_MAG-GUT42494.fa</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
+        <v>102461.0152130505</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -648,21 +619,18 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT41924.fa</t>
+          <t>even_MAG-GUT42584.fa</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
+        <v>81549.14162279168</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -671,21 +639,18 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT42485.fa</t>
+          <t>even_MAG-GUT43894.fa</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
+        <v>81832.4187264478</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -694,21 +659,18 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT42494.fa</t>
+          <t>even_MAG-GUT52107.fa</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
+        <v>116802.7749086313</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -717,21 +679,18 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT42584.fa</t>
+          <t>even_MAG-GUT5727.fa</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1</v>
+        <v>84473.23288990806</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D13" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -740,21 +699,18 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT43894.fa</t>
+          <t>even_MAG-GUT59039.fa</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1</v>
+        <v>77457.33608977369</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D14" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -763,21 +719,18 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT52107.fa</t>
+          <t>even_MAG-GUT61159.fa</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1</v>
+        <v>87885.79209551282</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D15" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -786,21 +739,18 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT52138.fa</t>
+          <t>even_MAG-GUT61959.fa</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1</v>
+        <v>89277.35330399006</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D16" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -809,21 +759,18 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT5727.fa</t>
+          <t>even_MAG-GUT70200.fa</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1</v>
+        <v>114961.8156116052</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D17" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -832,21 +779,18 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT59039.fa</t>
+          <t>even_MAG-GUT77982.fa</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1</v>
+        <v>105234.9571069992</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D18" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -855,21 +799,18 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT61159.fa</t>
+          <t>even_MAG-GUT78879.fa</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1</v>
+        <v>113890.5585103906</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D19" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -878,21 +819,18 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT61959.fa</t>
+          <t>even_MAG-GUT78908.fa</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1</v>
+        <v>93748.30563322347</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D20" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -901,21 +839,18 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT70200.fa</t>
+          <t>even_MAG-GUT83946.fa</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1</v>
+        <v>91274.61671756732</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D21" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -924,21 +859,18 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT77982.fa</t>
+          <t>even_MAG-GUT86868.fa</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
+        <v>107439.9103055472</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D22" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -947,21 +879,18 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT78879.fa</t>
+          <t>even_MAG-GUT87091.fa</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" t="n">
-        <v>1</v>
+        <v>117380.4233117023</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D23" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -970,21 +899,18 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT78908.fa</t>
+          <t>even_MAG-GUT87486.fa</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1</v>
+        <v>118380.9714551817</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D24" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -993,21 +919,18 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT83946.fa</t>
+          <t>even_MAG-GUT87573.fa</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1</v>
+        <v>118498.23652985</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D25" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -1016,21 +939,18 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT84692.fa</t>
+          <t>even_MAG-GUT87828.fa</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" t="n">
-        <v>1</v>
+        <v>118957.9554701441</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D26" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -1039,21 +959,18 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT85846.fa</t>
+          <t>even_MAG-GUT88085.fa</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" t="n">
-        <v>1</v>
+        <v>123162.7889049486</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D27" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -1062,21 +979,18 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT86514.fa</t>
+          <t>even_MAG-GUT88218.fa</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" t="n">
-        <v>1</v>
+        <v>120740.43272986</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D28" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -1085,21 +999,18 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT86868.fa</t>
+          <t>even_MAG-GUT88257.fa</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" t="n">
-        <v>1</v>
+        <v>112605.7526683244</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D29" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -1108,21 +1019,18 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT87091.fa</t>
+          <t>even_MAG-GUT88679.fa</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" t="n">
-        <v>1</v>
+        <v>112176.3614426853</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D30" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>
@@ -1131,182 +1039,18 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT87486.fa</t>
+          <t>even_MAG-GUT88862.fa</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" t="n">
-        <v>1</v>
+        <v>113033.5730537835</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>o__Christensenellales</t>
+        </is>
       </c>
       <c r="D31" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT87573.fa</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" t="n">
-        <v>1</v>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT87828.fa</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT88085.fa</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" t="n">
-        <v>1</v>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT88218.fa</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT88257.fa</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" t="n">
-        <v>1</v>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT88679.fa</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" t="n">
-        <v>1</v>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT88862.fa</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>1</v>
-      </c>
-      <c r="C38" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>o__Christensenellales</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
         <is>
           <t>o__Christensenellales</t>
         </is>

</xml_diff>